<commit_message>
queue admin mails, delete book
and more ui streamlining
</commit_message>
<xml_diff>
--- a/devNotes/mockUps.xlsx
+++ b/devNotes/mockUps.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="19095" windowHeight="12015" tabRatio="245" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="15270" windowHeight="5685" tabRatio="347" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ResetPassword" sheetId="1" r:id="rId1"/>
     <sheet name="Add Books" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Admin Tasks" sheetId="3" r:id="rId3"/>
+    <sheet name="Delete Book" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="130">
   <si>
     <t>User Forgot Password</t>
   </si>
@@ -366,6 +367,69 @@
   </si>
   <si>
     <t>FlatBook-&gt;suggestCategories($categories)</t>
+  </si>
+  <si>
+    <t>When new user joins</t>
+  </si>
+  <si>
+    <t>If user from new location, add data to location table, add locationid to user table</t>
+  </si>
+  <si>
+    <t>If user has already added book, add locationid to bookcopy</t>
+  </si>
+  <si>
+    <t>When user adds book</t>
+  </si>
+  <si>
+    <t>Verify book and update checked flag</t>
+  </si>
+  <si>
+    <t>Verify category, add in bookcategory if required</t>
+  </si>
+  <si>
+    <t>When user suggests category</t>
+  </si>
+  <si>
+    <t>Add new category if appropriate and add record in bookcopies</t>
+  </si>
+  <si>
+    <t>When user deletes book</t>
+  </si>
+  <si>
+    <t>Verify what information has been deleted and actually delete from tables (transactions, messages, bookcopies, books)</t>
+  </si>
+  <si>
+    <t>BookCopy-&gt;delete()</t>
+  </si>
+  <si>
+    <t>Verify that no active transactions exist</t>
+  </si>
+  <si>
+    <t>If they do, give user details of transaction and ask for confirmation</t>
+  </si>
+  <si>
+    <t>If they do not, ask user for plain confirmation</t>
+  </si>
+  <si>
+    <t>If confirmed</t>
+  </si>
+  <si>
+    <t>Mark bookcopy deleted</t>
+  </si>
+  <si>
+    <t>If no more copy of this book</t>
+  </si>
+  <si>
+    <t>Mark bookcategory as deleted</t>
+  </si>
+  <si>
+    <t>Mark book deleted</t>
+  </si>
+  <si>
+    <t>Send mail to admin about deletion</t>
+  </si>
+  <si>
+    <t>Mark transactions and messages deleted - if they exist</t>
   </si>
 </sst>
 </file>
@@ -2884,8 +2948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:AT59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="O59" sqref="O59"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4612,12 +4676,145 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18.75">
+      <c r="A1" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18.75">
+      <c r="A5" s="22" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="18.75">
+      <c r="A9" s="22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="18.75">
+      <c r="A12" s="22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75">
+      <c r="A1" s="22" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="21"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="21"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="21"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="21"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="C10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="C11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
record total in browse
</commit_message>
<xml_diff>
--- a/devNotes/mockUps.xlsx
+++ b/devNotes/mockUps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="15270" windowHeight="5685" tabRatio="347" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="15270" windowHeight="5685" tabRatio="347" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ResetPassword" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Admin Tasks" sheetId="3" r:id="rId3"/>
     <sheet name="Delete Book" sheetId="4" r:id="rId4"/>
     <sheet name="Blog" sheetId="5" r:id="rId5"/>
+    <sheet name="Ways To Borrow" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="176">
   <si>
     <t>User Forgot Password</t>
   </si>
@@ -528,12 +529,54 @@
   <si>
     <t>CategorySlug</t>
   </si>
+  <si>
+    <t>Library Name</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Within City</t>
+  </si>
+  <si>
+    <t>Within Country</t>
+  </si>
+  <si>
+    <t>International</t>
+  </si>
+  <si>
+    <t>Meet In Person</t>
+  </si>
+  <si>
+    <t>Ways to Borrow / Take Away</t>
+  </si>
+  <si>
+    <t>I can deliver</t>
+  </si>
+  <si>
+    <t>You can have it collected</t>
+  </si>
+  <si>
+    <t>I will post</t>
+  </si>
+  <si>
+    <t>You post back</t>
+  </si>
+  <si>
+    <t>I will post books for give away</t>
+  </si>
+  <si>
+    <t>You pay for shipping</t>
+  </si>
+  <si>
+    <t>Find out postage costs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -592,6 +635,14 @@
       <u/>
       <sz val="11"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -841,7 +892,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -896,6 +947,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4930,7 +4990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
@@ -5095,4 +5155,87 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="F2:J12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="11" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="6:10" ht="21">
+      <c r="H2" s="49" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="6:10">
+      <c r="H3" s="48" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="6:10">
+      <c r="H5" s="50" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="6:10">
+      <c r="H6" s="48"/>
+    </row>
+    <row r="7" spans="6:10">
+      <c r="F7" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="H7" s="50" t="s">
+        <v>165</v>
+      </c>
+      <c r="J7" s="50" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="6:10">
+      <c r="F8" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="H8" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="J8" s="48" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="6:10">
+      <c r="F9" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="H9" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="J9" s="48" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="6:10">
+      <c r="F10" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="H10" s="48" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="6:10">
+      <c r="H12" s="48" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>